<commit_message>
update excel cost tracking sheet
</commit_message>
<xml_diff>
--- a/testing_equipment/cost_tracking.xlsx
+++ b/testing_equipment/cost_tracking.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\testing_equipment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5091143-C615-4751-B8DD-DF6B2A3EB23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652F9650-88D2-4A86-ACB5-B62D6760D9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Overall" sheetId="1" r:id="rId1"/>
     <sheet name="Per Unit" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Project Overall'!$D$1:$D$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Item</t>
   </si>
@@ -130,7 +133,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Total Project Time (days)</t>
+    <t>Cost/Day</t>
+  </si>
+  <si>
+    <t>Project Length (days)</t>
   </si>
 </sst>
 </file>
@@ -165,12 +171,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -179,7 +200,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -197,6 +218,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -479,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,48 +524,52 @@
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>19.239999999999998</v>
+        <v>33.9</v>
       </c>
       <c r="D2" s="6">
-        <v>45339</v>
+        <v>45337</v>
       </c>
       <c r="E2" s="2">
         <f>SUM(C:C)</f>
-        <v>342.71</v>
+        <v>342.71000000000004</v>
       </c>
       <c r="F2" s="8">
         <f>ROUNDUP(E2/50,0)</f>
@@ -542,52 +577,56 @@
       </c>
       <c r="H2" s="7">
         <f>D10-D2</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="I2" s="9">
+        <f>E2/H2</f>
+        <v>8.3587804878048786</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1">
-        <v>33.9</v>
+        <v>55</v>
       </c>
       <c r="D3" s="6">
         <v>45337</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="D4" s="6">
+        <v>45339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>42.8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="6">
         <v>45357</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1">
-        <v>59.7</v>
-      </c>
-      <c r="D5" s="6">
-        <v>45363</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -601,7 +640,7 @@
         <v>45358</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -615,35 +654,35 @@
         <v>45362</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1">
+        <v>59.7</v>
+      </c>
+      <c r="D8" s="6">
+        <v>45363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>54.49</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="6">
         <v>45378</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1">
-        <v>55</v>
-      </c>
-      <c r="D9" s="6">
-        <v>45337</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -658,6 +697,10 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D10" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F10">
+    <sortCondition ref="D2:D10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -666,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C094F0E-38F2-4E31-A708-722C58BEC856}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,19 +721,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="11" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>